<commit_message>
DisableSubtotalLine + correct style of grouped and merged cells Correct Break Right Groups according on left groups Ends without Subtotal lines
# Conflicts:
#	tests/Gauges/GroupTagTests_DisableSubTotals_MergeLabels.xlsx
#	tests/Templates/GroupTagTests_DisableSubTotals_MergeLabels.xlsx
</commit_message>
<xml_diff>
--- a/tests/Templates/GroupTagTests_DisableSubTotals_MergeLabels.xlsx
+++ b/tests/Templates/GroupTagTests_DisableSubTotals_MergeLabels.xlsx
@@ -86,13 +86,13 @@
     <t>{{item.Terms}}</t>
   </si>
   <si>
+    <t>&lt;&lt;group MergeLabels=Merge2 labelformat="Total For {0}:" &gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;&lt;group MergeLabels=Merge2  labelformat="Total By Payment  {0}:"&gt;&gt;</t>
+  </si>
+  <si>
     <t>&lt;&lt;group MergeLabels=Merge2 DisableSubtotalLine&gt;&gt;</t>
-  </si>
-  <si>
-    <t>&lt;&lt;group MergeLabels=Merge2 labelformat="Total For {0}:" &gt;&gt;</t>
-  </si>
-  <si>
-    <t>&lt;&lt;group MergeLabels=Merge2  labelformat="Total By Payment  {0}:"&gt;&gt;</t>
   </si>
 </sst>
 </file>
@@ -800,7 +800,7 @@
   <sheetViews>
     <sheetView showZeros="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
+      <selection pane="bottomLeft" activeCell="L35" sqref="L35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -916,13 +916,13 @@
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="25"/>
       <c r="B6" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="13" t="s">
         <v>22</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>23</v>
       </c>
       <c r="E6" s="14"/>
       <c r="F6" s="15"/>

</xml_diff>